<commit_message>
add thaiid to export
</commit_message>
<xml_diff>
--- a/wwwroot/GatewayExcel/InputTemplate/GatewayTransaction.xlsx
+++ b/wwwroot/GatewayExcel/InputTemplate/GatewayTransaction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\SLA_Management\wwwroot\GatewayExcel\InputTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3666560-76AC-4FF4-AA2C-E831F23846BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0837863D-FFD0-4B2E-BFCB-A7D01FA1DB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="345" windowWidth="19875" windowHeight="7725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$H$7</definedName>
   </definedNames>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>จากวันที่</t>
   </si>
@@ -60,7 +60,10 @@
     <t>ID</t>
   </si>
   <si>
-    <t>SeqNo</t>
+    <t>Seq No</t>
+  </si>
+  <si>
+    <t>Thai ID</t>
   </si>
   <si>
     <t>PhoneOTP</t>
@@ -499,28 +502,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L7"/>
+  <dimension ref="A2:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="6" width="11.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="2" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="7" width="11.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="18">
+    <row r="2" spans="1:13" ht="18">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -530,8 +533,9 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="18">
+    <row r="3" spans="1:13" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -541,30 +545,31 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="7"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15">
+    <row r="4" spans="1:13" ht="15">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15">
+    <row r="5" spans="1:13" ht="15">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="33">
+    <row r="7" spans="1:13" ht="33">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -574,7 +579,7 @@
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -583,13 +588,13 @@
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="6" t="s">
@@ -597,12 +602,15 @@
       </c>
       <c r="K7" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="63" orientation="portrait" r:id="rId1"/>

</xml_diff>